<commit_message>
working on batch management; finish upload xlsx; add angular material module
</commit_message>
<xml_diff>
--- a/kuaidi-front/src/assets/new.xlsx
+++ b/kuaidi-front/src/assets/new.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cocoastarrion/KudiDi/kuaidi-front/src/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33256C83-CC4A-0543-9D05-DC5FCDFB2F8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4A8DC7-09E4-7748-B03E-43126ACA22B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41480" yWindow="4560" windowWidth="28040" windowHeight="17040" xr2:uid="{2B55E797-03F9-4241-A045-4D4795F6B3EF}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>序号</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>6260003333</t>
+  </si>
+  <si>
+    <t>22</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,6 +771,9 @@
       <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
+      <c r="I4" s="2" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>